<commit_message>
Added Core SW pin mapping (from Spark-Wiring)
</commit_message>
<xml_diff>
--- a/Pin mapping/core-pin-mapping-v008.xlsx
+++ b/Pin mapping/core-pin-mapping-v008.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$49</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="198">
   <si>
     <t>1_MOSI</t>
   </si>
@@ -517,9 +517,6 @@
     <t>STM Pin #</t>
   </si>
   <si>
-    <t>Core</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
@@ -614,6 +611,12 @@
   </si>
   <si>
     <t>BTN</t>
+  </si>
+  <si>
+    <t>Core SW</t>
+  </si>
+  <si>
+    <t>Core HW</t>
   </si>
 </sst>
 </file>
@@ -1138,18 +1141,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="12" max="12" width="31" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1184,10 +1187,13 @@
         <v>163</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>197</v>
+      </c>
+      <c r="M1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>70</v>
       </c>
@@ -1212,10 +1218,13 @@
         <v>10</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>166</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>66</v>
       </c>
@@ -1240,10 +1249,13 @@
         <v>11</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>167</v>
+      </c>
+      <c r="M3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>62</v>
       </c>
@@ -1268,10 +1280,13 @@
         <v>12</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>164</v>
+      </c>
+      <c r="M4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>58</v>
       </c>
@@ -1296,10 +1311,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>165</v>
+      </c>
+      <c r="M5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -1324,10 +1342,13 @@
         <v>14</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>168</v>
+      </c>
+      <c r="M6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1350,10 +1371,13 @@
         <v>15</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>169</v>
+      </c>
+      <c r="M7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>46</v>
       </c>
@@ -1378,10 +1402,13 @@
         <v>16</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>170</v>
+      </c>
+      <c r="M8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -1406,10 +1433,13 @@
         <v>17</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>171</v>
+      </c>
+      <c r="M9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
         <v>107</v>
       </c>
@@ -1436,10 +1466,13 @@
         <v>29</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>181</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
         <v>105</v>
       </c>
@@ -1464,10 +1497,13 @@
         <v>30</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>182</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
         <v>103</v>
       </c>
@@ -1492,10 +1528,13 @@
         <v>31</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>195</v>
+      </c>
+      <c r="M12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
         <v>101</v>
       </c>
@@ -1522,10 +1561,10 @@
         <v>32</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
         <v>99</v>
       </c>
@@ -1552,10 +1591,10 @@
         <v>33</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
         <v>97</v>
       </c>
@@ -1580,8 +1619,11 @@
       <c r="L15" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="3" t="s">
         <v>95</v>
       </c>
@@ -1606,8 +1648,11 @@
       <c r="L16" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
         <v>93</v>
       </c>
@@ -1632,8 +1677,11 @@
       <c r="L17" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1656,10 +1704,13 @@
         <v>18</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>172</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="3" t="s">
         <v>128</v>
       </c>
@@ -1682,10 +1733,13 @@
         <v>19</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>173</v>
+      </c>
+      <c r="M19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -1708,7 +1762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1733,8 +1787,11 @@
       <c r="L21" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="3" t="s">
         <v>89</v>
       </c>
@@ -1759,8 +1816,11 @@
       <c r="L22" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -1783,8 +1843,11 @@
       <c r="L23" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
         <v>84</v>
       </c>
@@ -1793,7 +1856,7 @@
         <v>85</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1811,8 +1874,11 @@
       <c r="L24" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>80</v>
       </c>
@@ -1839,8 +1905,11 @@
       <c r="L25" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="3" t="s">
         <v>126</v>
       </c>
@@ -1863,10 +1932,10 @@
         <v>45</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
         <v>141</v>
       </c>
@@ -1887,10 +1956,10 @@
         <v>46</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -1915,10 +1984,10 @@
         <v>21</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -1943,10 +2012,10 @@
         <v>22</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="3" t="s">
         <v>120</v>
       </c>
@@ -1975,10 +2044,10 @@
         <v>25</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>116</v>
       </c>
@@ -2003,10 +2072,10 @@
         <v>26</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>112</v>
       </c>
@@ -2031,7 +2100,7 @@
         <v>27</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2057,7 +2126,7 @@
         <v>28</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2128,7 +2197,7 @@
         <v>5</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2142,7 +2211,7 @@
         <v>6</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2167,7 +2236,7 @@
         <v>7</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2297,7 +2366,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K49"/>
+  <autoFilter ref="A1:M49"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="gpio"/>
     <hyperlink ref="B1" r:id="rId2" location="adc"/>
@@ -2366,13 +2435,13 @@
     <row r="3" spans="2:13">
       <c r="B3" s="8"/>
       <c r="C3" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>190</v>
-      </c>
       <c r="E3" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>20</v>
@@ -2403,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
@@ -2439,7 +2508,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>62</v>
@@ -2480,7 +2549,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>58</v>
@@ -2521,7 +2590,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>128</v>
@@ -2562,7 +2631,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>38</v>
@@ -2603,7 +2672,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>42</v>
@@ -2644,7 +2713,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>46</v>
@@ -2685,7 +2754,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>50</v>
@@ -2726,7 +2795,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>53</v>
@@ -2767,7 +2836,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>66</v>
@@ -2808,7 +2877,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>70</v>
@@ -3213,7 +3282,7 @@
         <v>23</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -3231,7 +3300,7 @@
         <v>24</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>

</xml_diff>